<commit_message>
Small fix to correctly deal with PP-g-MAH layers and mixedPO streams
</commit_message>
<xml_diff>
--- a/tables/CEFLEX D4ACE July 2025.xlsx
+++ b/tables/CEFLEX D4ACE July 2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emergingmotif-my.sharepoint.com/personal/dennis_bankmann_emergingmotif_com/Documents/Clients/CEFLEX/Score calculator/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emergingmotif-my.sharepoint.com/personal/dennis_bankmann_emergingmotif_com/Documents/Clients/CEFLEX/recyclability-score-simulation-tool/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="586" documentId="8_{5D1E29AC-F520-484B-A306-57C8DBE8C32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1C4B180-93CE-D846-8184-27D6A2A7E3DF}"/>
+  <xr:revisionPtr revIDLastSave="590" documentId="8_{5D1E29AC-F520-484B-A306-57C8DBE8C32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB828ADD-97D6-824F-BC9D-4509CEF246C5}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="760" windowWidth="28260" windowHeight="18360" activeTab="3" xr2:uid="{FB9E261B-E538-6849-9602-3C54F79805DE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28260" windowHeight="18360" activeTab="1" xr2:uid="{FB9E261B-E538-6849-9602-3C54F79805DE}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="79">
   <si>
     <t>Material</t>
   </si>
@@ -345,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -355,8 +355,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,10 +370,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -769,258 +763,258 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20">
         <v>100</v>
       </c>
     </row>
@@ -1031,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{896C7AD7-2029-2145-B988-B51E76C18261}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1120,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -1140,7 +1134,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>100</v>
@@ -1153,15 +1147,12 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
         <v>100</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1170,287 +1161,270 @@
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
         <v>100</v>
       </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5">
-        <v>5</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="5">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="5">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="5">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="5">
-        <v>5</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="5">
-        <v>5</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="C14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="5">
-        <v>5</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="5">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="5">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="5">
-        <v>5</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="I18" t="s">
-        <v>69</v>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="5">
-        <v>5</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="5">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="5">
-        <v>5</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="5">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="5">
-        <v>5</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="5">
-        <v>5</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="D25">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1462,7 +1436,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,448 +1506,398 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>100</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4">
         <v>100</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="1">
         <v>100</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>100</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7">
         <v>10</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8">
         <v>40</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9">
         <v>40</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>100</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11">
         <v>100</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12">
         <v>100</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13">
         <v>100</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14">
         <v>100</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15">
         <v>100</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16">
         <v>35</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>0</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17">
         <v>20</v>
       </c>
-      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18">
         <v>20</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18">
         <v>20</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18">
         <v>35</v>
       </c>
-      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="5">
-        <v>5</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="D19">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="5">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="D20">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="5">
-        <v>5</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
+      <c r="D21">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="5">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="D22">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="5">
-        <v>5</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="D23">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24">
         <v>10</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="5" t="s">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="5">
-        <v>5</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="D25">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="5" t="s">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="5">
-        <v>5</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
+      <c r="D26">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="5">
-        <v>5</v>
-      </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="D27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="5">
-        <v>5</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="D28">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29">
         <v>3</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29">
         <v>3</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29">
         <v>5</v>
       </c>
       <c r="I29" t="s">
@@ -1981,96 +1905,86 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="5">
-        <v>5</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="D30">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
         <v>72</v>
       </c>
-      <c r="D31" s="5">
-        <v>5</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="D31">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="5">
-        <v>5</v>
-      </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="D32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="5">
-        <v>5</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="D33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="5">
-        <v>5</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="D34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35">
         <v>5</v>
       </c>
     </row>
@@ -2081,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2B07F74-6BE2-4A47-B287-A2C3838A2311}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2155,329 +2069,304 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3">
         <v>100</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5">
+      <c r="E6">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F6">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="5">
-        <v>5</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="5">
-        <v>5</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="5">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="D10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="5">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D12">
         <v>7</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="5">
-        <v>5</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="5">
-        <v>5</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="5">
-        <v>5</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="I16" t="s">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="5">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="5">
-        <v>5</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="5">
-        <v>5</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="5">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="5">
-        <v>5</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="5">
-        <v>5</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="D23">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>